<commit_message>
EPBDS - tests extended: references on array
</commit_message>
<xml_diff>
--- a/POI/trunk/org.openl.lib.poi35.dev.modified/test/resources/ArrayFormulaFunctions.xlsx
+++ b/POI/trunk/org.openl.lib.poi35.dev.modified/test/resources/ArrayFormulaFunctions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Array Formula  Functions Test</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>column on array</t>
+  </si>
+  <si>
+    <t>Use array cell</t>
+  </si>
+  <si>
+    <t>ref array in array</t>
   </si>
 </sst>
 </file>
@@ -434,13 +440,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N101"/>
+  <dimension ref="A1:N110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="N89" sqref="N89"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="J103" sqref="J103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="G1" t="s">
@@ -935,8 +944,8 @@
     </row>
     <row r="75" spans="1:14">
       <c r="C75">
-        <f t="array" ref="C75">SUM(IF(A67:B68&gt;2,A67:B68))</f>
-        <v>7</v>
+        <f t="array" ref="C75">SUM(IF(A67:B68&gt;2,A67:B68,1))</f>
+        <v>9</v>
       </c>
       <c r="I75">
         <v>7</v>
@@ -1091,8 +1100,72 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="8:8">
-      <c r="H101" t="s">
+    <row r="97" spans="1:14">
+      <c r="A97">
+        <f t="array" ref="A97:B98">SQRT({1,2;3,4})</f>
+        <v>1</v>
+      </c>
+      <c r="B97">
+        <v>1.4142135623730951</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14">
+      <c r="A98">
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="B98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14">
+      <c r="C99">
+        <f>B98+1</f>
+        <v>3</v>
+      </c>
+      <c r="I99">
+        <v>3</v>
+      </c>
+      <c r="N99" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14">
+      <c r="B102">
+        <f t="array" ref="B102:C103">A97:B98+1</f>
+        <v>2</v>
+      </c>
+      <c r="C102">
+        <v>2.4142135623730949</v>
+      </c>
+      <c r="I102">
+        <v>2</v>
+      </c>
+      <c r="J102">
+        <v>2.4142135623730949</v>
+      </c>
+      <c r="N102" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14">
+      <c r="B103">
+        <v>2.7320508075688772</v>
+      </c>
+      <c r="C103">
+        <v>3</v>
+      </c>
+      <c r="I103">
+        <v>2.7320508075688772</v>
+      </c>
+      <c r="J103">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14">
+      <c r="H110" t="s">
+        <v>2</v>
+      </c>
+      <c r="I110" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EPBDS - if fixed
</commit_message>
<xml_diff>
--- a/POI/trunk/org.openl.lib.poi35.dev.modified/test/resources/ArrayFormulaFunctions.xlsx
+++ b/POI/trunk/org.openl.lib.poi35.dev.modified/test/resources/ArrayFormulaFunctions.xlsx
@@ -442,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="J103" sqref="J103"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="I75" sqref="I75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -948,7 +948,7 @@
         <v>9</v>
       </c>
       <c r="I75">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N75" t="s">
         <v>22</v>

</xml_diff>